<commit_message>
vault backup: 2025-03-14 12:54:17
</commit_message>
<xml_diff>
--- a/РАбОТА/Списание/Списание Ноутбуки.xlsx
+++ b/РАбОТА/Списание/Списание Ноутбуки.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,13 +9,69 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+  <si>
+    <t>Сотрудник</t>
+  </si>
+  <si>
+    <t>Модель</t>
+  </si>
+  <si>
+    <t>S\N (серийный номер)</t>
+  </si>
+  <si>
+    <t>Молодцов Д.В.</t>
+  </si>
+  <si>
+    <t>ASUS X4250LN-WX034H</t>
+  </si>
+  <si>
+    <t>E4N0CX62583416A</t>
+  </si>
+  <si>
+    <t>Родин Вадим</t>
+  </si>
+  <si>
+    <t>Eee PC 1201NL</t>
+  </si>
+  <si>
+    <t>A8OAAS275632</t>
+  </si>
+  <si>
+    <t>Варибус П.И.</t>
+  </si>
+  <si>
+    <t>R61e</t>
+  </si>
+  <si>
+    <t>L3-ER768</t>
+  </si>
+  <si>
+    <t>Comqaq 6715s</t>
+  </si>
+  <si>
+    <t>CNU7450DTY8</t>
+  </si>
+  <si>
+    <t>Лазарев Ю.П.</t>
+  </si>
+  <si>
+    <t>ASUS K-43S</t>
+  </si>
+  <si>
+    <t>EAN0CV006011418</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,17 +104,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -96,9 +160,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +197,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -168,7 +232,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -341,13 +405,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2025-03-14 12:56:15
</commit_message>
<xml_diff>
--- a/РАбОТА/Списание/Списание Ноутбуки.xlsx
+++ b/РАбОТА/Списание/Списание Ноутбуки.xlsx
@@ -71,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,16 +79,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -96,12 +111,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -409,7 +445,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,73 +455,74 @@
     <col min="3" max="3" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2025-03-14 12:58:41
</commit_message>
<xml_diff>
--- a/РАбОТА/Списание/Списание Ноутбуки.xlsx
+++ b/РАбОТА/Списание/Списание Ноутбуки.xlsx
@@ -37,9 +37,6 @@
     <t>Родин Вадим</t>
   </si>
   <si>
-    <t>Eee PC 1201NL</t>
-  </si>
-  <si>
     <t>A8OAAS275632</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>EAN0CV006011418</t>
+  </si>
+  <si>
+    <t>ASUS Eee PC 1201NL</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,43 +482,43 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2025-03-14 13:02:01
</commit_message>
<xml_diff>
--- a/РАбОТА/Списание/Списание Ноутбуки.xlsx
+++ b/РАбОТА/Списание/Списание Ноутбуки.xlsx
@@ -43,9 +43,6 @@
     <t>Варибус П.И.</t>
   </si>
   <si>
-    <t>R61e</t>
-  </si>
-  <si>
     <t>L3-ER768</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>ASUS Eee PC 1201NL</t>
+  </si>
+  <si>
+    <t>Lenovo ThinkPad R61e</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +482,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -493,10 +493,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -504,21 +504,21 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>